<commit_message>
Crutched some new data for approximation methods.
</commit_message>
<xml_diff>
--- a/results/datasetNearOne_polytree15.xlsx
+++ b/results/datasetNearOne_polytree15.xlsx
@@ -466,13 +466,13 @@
         <v>25</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02300000000000002</v>
+        <v>0.01900000000000002</v>
       </c>
       <c r="E2" t="n">
-        <v>0.977</v>
+        <v>0.981</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1126666069030762</v>
+        <v>0.1154937744140625</v>
       </c>
     </row>
     <row r="3">
@@ -488,13 +488,13 @@
         <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01700000000000002</v>
+        <v>0.02300000000000002</v>
       </c>
       <c r="E3" t="n">
-        <v>0.983</v>
+        <v>0.977</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1249744892120361</v>
+        <v>0.1201694011688232</v>
       </c>
     </row>
     <row r="4">
@@ -510,13 +510,13 @@
         <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01700000000000002</v>
+        <v>0.01900000000000002</v>
       </c>
       <c r="E4" t="n">
-        <v>0.983</v>
+        <v>0.981</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1249210834503174</v>
+        <v>0.1318693161010742</v>
       </c>
     </row>
     <row r="5">
@@ -532,13 +532,13 @@
         <v>25</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02300000000000002</v>
+        <v>0.01400000000000002</v>
       </c>
       <c r="E5" t="n">
-        <v>0.977</v>
+        <v>0.9859999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1250159740447998</v>
+        <v>0.1320602893829346</v>
       </c>
     </row>
     <row r="6">
@@ -554,13 +554,13 @@
         <v>25</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02100000000000002</v>
+        <v>0.01800000000000002</v>
       </c>
       <c r="E6" t="n">
-        <v>0.979</v>
+        <v>0.9819999999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1249701976776123</v>
+        <v>0.1213304996490479</v>
       </c>
     </row>
     <row r="7">
@@ -576,13 +576,13 @@
         <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01800000000000002</v>
+        <v>0.01500000000000002</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9819999999999999</v>
+        <v>0.985</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1244974136352539</v>
+        <v>0.1312618255615234</v>
       </c>
     </row>
     <row r="8">
@@ -598,13 +598,13 @@
         <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01800000000000002</v>
+        <v>0.02100000000000002</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9819999999999999</v>
+        <v>0.979</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1250126361846924</v>
+        <v>0.1224386692047119</v>
       </c>
     </row>
     <row r="9">
@@ -620,13 +620,13 @@
         <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01900000000000002</v>
+        <v>0.01700000000000002</v>
       </c>
       <c r="E9" t="n">
-        <v>0.981</v>
+        <v>0.983</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1249756813049316</v>
+        <v>0.1228210926055908</v>
       </c>
     </row>
     <row r="10">
@@ -642,13 +642,13 @@
         <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01900000000000002</v>
+        <v>0.01200000000000002</v>
       </c>
       <c r="E10" t="n">
-        <v>0.981</v>
+        <v>0.988</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1249716281890869</v>
+        <v>0.132476806640625</v>
       </c>
     </row>
     <row r="11">
@@ -664,13 +664,13 @@
         <v>25</v>
       </c>
       <c r="D11" t="n">
-        <v>0.02300000000000002</v>
+        <v>0.01800000000000002</v>
       </c>
       <c r="E11" t="n">
-        <v>0.977</v>
+        <v>0.9819999999999999</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1405458450317383</v>
+        <v>0.169569730758667</v>
       </c>
     </row>
     <row r="12">
@@ -686,13 +686,13 @@
         <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02300000000000002</v>
+        <v>0.01500000000000002</v>
       </c>
       <c r="E12" t="n">
-        <v>0.977</v>
+        <v>0.985</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1319265365600586</v>
+        <v>0.1316366195678711</v>
       </c>
     </row>
     <row r="13">
@@ -708,13 +708,13 @@
         <v>25</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02200000000000002</v>
+        <v>0.02500000000000002</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9779999999999999</v>
+        <v>0.975</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1338682174682617</v>
+        <v>0.124767541885376</v>
       </c>
     </row>
     <row r="14">
@@ -730,13 +730,13 @@
         <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02700000000000002</v>
+        <v>0.02900000000000002</v>
       </c>
       <c r="E14" t="n">
-        <v>0.973</v>
+        <v>0.9710000000000001</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1258747577667236</v>
+        <v>0.1298635005950928</v>
       </c>
     </row>
     <row r="15">
@@ -752,13 +752,13 @@
         <v>25</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01500000000000002</v>
+        <v>0.02000000000000002</v>
       </c>
       <c r="E15" t="n">
-        <v>0.985</v>
+        <v>0.98</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1194002628326416</v>
+        <v>0.1295702457427979</v>
       </c>
     </row>
     <row r="16">
@@ -774,13 +774,13 @@
         <v>25</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01100000000000002</v>
+        <v>0.01400000000000002</v>
       </c>
       <c r="E16" t="n">
-        <v>0.989</v>
+        <v>0.9859999999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1217951774597168</v>
+        <v>0.1240003108978271</v>
       </c>
     </row>
     <row r="17">
@@ -796,13 +796,13 @@
         <v>25</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02700000000000002</v>
+        <v>0.01400000000000002</v>
       </c>
       <c r="E17" t="n">
-        <v>0.973</v>
+        <v>0.9859999999999999</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1249825954437256</v>
+        <v>0.122389554977417</v>
       </c>
     </row>
     <row r="18">
@@ -818,13 +818,13 @@
         <v>25</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02200000000000002</v>
+        <v>0.01900000000000002</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9779999999999999</v>
+        <v>0.981</v>
       </c>
       <c r="F18" t="n">
-        <v>0.124974250793457</v>
+        <v>0.1262757778167725</v>
       </c>
     </row>
     <row r="19">
@@ -840,13 +840,13 @@
         <v>25</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01900000000000002</v>
+        <v>0.02200000000000002</v>
       </c>
       <c r="E19" t="n">
-        <v>0.981</v>
+        <v>0.9779999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1249716281890869</v>
+        <v>0.1187272071838379</v>
       </c>
     </row>
     <row r="20">
@@ -862,13 +862,13 @@
         <v>25</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01400000000000002</v>
+        <v>0.01500000000000002</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9859999999999999</v>
+        <v>0.985</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1249709129333496</v>
+        <v>0.1293425559997559</v>
       </c>
     </row>
     <row r="21">
@@ -890,7 +890,7 @@
         <v>0.984</v>
       </c>
       <c r="F21" t="n">
-        <v>0.12497878074646</v>
+        <v>0.1243667602539062</v>
       </c>
     </row>
     <row r="22">
@@ -906,13 +906,13 @@
         <v>25</v>
       </c>
       <c r="D22" t="n">
-        <v>0.02500000000000002</v>
+        <v>0.01900000000000002</v>
       </c>
       <c r="E22" t="n">
-        <v>0.975</v>
+        <v>0.981</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1093375682830811</v>
+        <v>0.1214327812194824</v>
       </c>
     </row>
     <row r="23">
@@ -928,13 +928,13 @@
         <v>25</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02000000000000002</v>
+        <v>0.02500000000000002</v>
       </c>
       <c r="E23" t="n">
-        <v>0.98</v>
+        <v>0.975</v>
       </c>
       <c r="F23" t="n">
-        <v>0.124957799911499</v>
+        <v>0.1222288608551025</v>
       </c>
     </row>
     <row r="24">
@@ -950,13 +950,13 @@
         <v>25</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02000000000000002</v>
+        <v>0.02600000000000002</v>
       </c>
       <c r="E24" t="n">
-        <v>0.98</v>
+        <v>0.974</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1249783039093018</v>
+        <v>0.1302516460418701</v>
       </c>
     </row>
     <row r="25">
@@ -972,13 +972,13 @@
         <v>25</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01700000000000002</v>
+        <v>0.01800000000000002</v>
       </c>
       <c r="E25" t="n">
-        <v>0.983</v>
+        <v>0.9819999999999999</v>
       </c>
       <c r="F25" t="n">
-        <v>0.124974250793457</v>
+        <v>0.1218783855438232</v>
       </c>
     </row>
     <row r="26">
@@ -994,13 +994,13 @@
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01900000000000002</v>
+        <v>0.01800000000000002</v>
       </c>
       <c r="E26" t="n">
-        <v>0.981</v>
+        <v>0.9819999999999999</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1249723434448242</v>
+        <v>0.1220965385437012</v>
       </c>
     </row>
     <row r="27">
@@ -1016,13 +1016,13 @@
         <v>25</v>
       </c>
       <c r="D27" t="n">
-        <v>0.09177066848945765</v>
+        <v>0.09815317668257657</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9082293315105423</v>
+        <v>0.9018468233174234</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1093518733978271</v>
+        <v>0.1236698627471924</v>
       </c>
     </row>
     <row r="28">
@@ -1038,13 +1038,13 @@
         <v>25</v>
       </c>
       <c r="D28" t="n">
-        <v>0.05568030066622866</v>
+        <v>0.07149487279737127</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9443196993337714</v>
+        <v>0.9285051272026287</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1249709129333496</v>
+        <v>0.1230001449584961</v>
       </c>
     </row>
     <row r="29">
@@ -1060,13 +1060,13 @@
         <v>25</v>
       </c>
       <c r="D29" t="n">
-        <v>0.04724073404440955</v>
+        <v>0.05870725233620675</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9527592659555904</v>
+        <v>0.9412927476637932</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1249654293060303</v>
+        <v>0.1215555667877197</v>
       </c>
     </row>
     <row r="30">
@@ -1082,13 +1082,13 @@
         <v>25</v>
       </c>
       <c r="D30" t="n">
-        <v>0.03919590627142523</v>
+        <v>0.04170526168787541</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9608040937285748</v>
+        <v>0.9582947383121245</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1249756813049316</v>
+        <v>0.1229496002197266</v>
       </c>
     </row>
     <row r="31">
@@ -1104,13 +1104,13 @@
         <v>25</v>
       </c>
       <c r="D31" t="n">
-        <v>0.07111570780296418</v>
+        <v>0.1379060306696481</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9288842921970358</v>
+        <v>0.862093969330352</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1249704360961914</v>
+        <v>0.1217947006225586</v>
       </c>
     </row>
     <row r="32">
@@ -1126,13 +1126,13 @@
         <v>25</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1011084886686431</v>
+        <v>0.1086603729347282</v>
       </c>
       <c r="E32" t="n">
-        <v>0.8988915113313568</v>
+        <v>0.8913396270652717</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1249706745147705</v>
+        <v>0.129378080368042</v>
       </c>
     </row>
     <row r="33">
@@ -1148,13 +1148,13 @@
         <v>25</v>
       </c>
       <c r="D33" t="n">
-        <v>0.07693500481922694</v>
+        <v>0.0352276390032667</v>
       </c>
       <c r="E33" t="n">
-        <v>0.923064995180773</v>
+        <v>0.9647723609967332</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1249706745147705</v>
+        <v>0.1235854625701904</v>
       </c>
     </row>
     <row r="34">
@@ -1170,13 +1170,13 @@
         <v>25</v>
       </c>
       <c r="D34" t="n">
-        <v>0.02839801399537676</v>
+        <v>0.09336999238232623</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9716019860046232</v>
+        <v>0.9066300076176738</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1249701976776123</v>
+        <v>0.1226158142089844</v>
       </c>
     </row>
     <row r="35">
@@ -1192,13 +1192,13 @@
         <v>25</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0494797801391642</v>
+        <v>0.06913463653283683</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9505202198608359</v>
+        <v>0.9308653634671632</v>
       </c>
       <c r="F35" t="n">
-        <v>0.1249711513519287</v>
+        <v>0.1317615509033203</v>
       </c>
     </row>
     <row r="36">
@@ -1214,13 +1214,13 @@
         <v>25</v>
       </c>
       <c r="D36" t="n">
-        <v>0.01862688554013893</v>
+        <v>0.03422218544281542</v>
       </c>
       <c r="E36" t="n">
-        <v>0.981373114459861</v>
+        <v>0.9657778145571845</v>
       </c>
       <c r="F36" t="n">
-        <v>0.1249704360961914</v>
+        <v>0.1213295459747314</v>
       </c>
     </row>
     <row r="37">
@@ -1236,13 +1236,13 @@
         <v>25</v>
       </c>
       <c r="D37" t="n">
-        <v>0.03915340188797786</v>
+        <v>0.1325327714541668</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9608465981120222</v>
+        <v>0.8674672285458332</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1249744892120361</v>
+        <v>0.1315577030181885</v>
       </c>
     </row>
     <row r="38">
@@ -1258,13 +1258,13 @@
         <v>25</v>
       </c>
       <c r="D38" t="n">
-        <v>0.05721134897020175</v>
+        <v>0.05871536912845587</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9427886510297984</v>
+        <v>0.9412846308715441</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1249666213989258</v>
+        <v>0.1217818260192871</v>
       </c>
     </row>
     <row r="39">
@@ -1280,13 +1280,13 @@
         <v>25</v>
       </c>
       <c r="D39" t="n">
-        <v>0.007029004844049813</v>
+        <v>0.05120872505066435</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9929709951559502</v>
+        <v>0.9487912749493356</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1249656677246094</v>
+        <v>0.1313879489898682</v>
       </c>
     </row>
     <row r="40">
@@ -1302,13 +1302,13 @@
         <v>25</v>
       </c>
       <c r="D40" t="n">
-        <v>0.09469139852696973</v>
+        <v>0.07222496627961045</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9053086014730303</v>
+        <v>0.9277750337203895</v>
       </c>
       <c r="F40" t="n">
-        <v>0.1249754428863525</v>
+        <v>0.1212751865386963</v>
       </c>
     </row>
     <row r="41">
@@ -1324,13 +1324,13 @@
         <v>25</v>
       </c>
       <c r="D41" t="n">
-        <v>0.05844594814807302</v>
+        <v>0.07305566223481794</v>
       </c>
       <c r="E41" t="n">
-        <v>0.941554051851927</v>
+        <v>0.926944337765182</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1249704360961914</v>
+        <v>0.1194047927856445</v>
       </c>
     </row>
     <row r="42">
@@ -1346,13 +1346,13 @@
         <v>25</v>
       </c>
       <c r="D42" t="n">
-        <v>0.06696473181780492</v>
+        <v>0.02997459196379001</v>
       </c>
       <c r="E42" t="n">
-        <v>0.9330352681821951</v>
+        <v>0.9700254080362101</v>
       </c>
       <c r="F42" t="n">
-        <v>0.124924898147583</v>
+        <v>0.1360173225402832</v>
       </c>
     </row>
     <row r="43">
@@ -1368,13 +1368,13 @@
         <v>25</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03227931147975124</v>
+        <v>0.1742881651531439</v>
       </c>
       <c r="E43" t="n">
-        <v>0.9677206885202488</v>
+        <v>0.8257118348468562</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1250114440917969</v>
+        <v>0.1174774169921875</v>
       </c>
     </row>
     <row r="44">
@@ -1390,13 +1390,13 @@
         <v>25</v>
       </c>
       <c r="D44" t="n">
-        <v>0.09341440612772921</v>
+        <v>0.05369779882569944</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9065855938722708</v>
+        <v>0.9463022011743005</v>
       </c>
       <c r="F44" t="n">
-        <v>0.1249299049377441</v>
+        <v>0.1333780288696289</v>
       </c>
     </row>
     <row r="45">
@@ -1412,13 +1412,13 @@
         <v>25</v>
       </c>
       <c r="D45" t="n">
-        <v>0.07097853749628664</v>
+        <v>0.08353488430538196</v>
       </c>
       <c r="E45" t="n">
-        <v>0.9290214625037134</v>
+        <v>0.916465115694618</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1250114440917969</v>
+        <v>0.121284008026123</v>
       </c>
     </row>
     <row r="46">
@@ -1434,13 +1434,13 @@
         <v>25</v>
       </c>
       <c r="D46" t="n">
-        <v>0.1439767232156074</v>
+        <v>0.09802387810758735</v>
       </c>
       <c r="E46" t="n">
-        <v>0.8560232767843926</v>
+        <v>0.9019761218924126</v>
       </c>
       <c r="F46" t="n">
-        <v>0.1093497276306152</v>
+        <v>0.1293256282806396</v>
       </c>
     </row>
     <row r="47">
@@ -1456,13 +1456,13 @@
         <v>25</v>
       </c>
       <c r="D47" t="n">
-        <v>0.02157907978304368</v>
+        <v>0.08952942608765634</v>
       </c>
       <c r="E47" t="n">
-        <v>0.9784209202169563</v>
+        <v>0.9104705739123437</v>
       </c>
       <c r="F47" t="n">
-        <v>0.1249713897705078</v>
+        <v>0.1241052150726318</v>
       </c>
     </row>
     <row r="48">
@@ -1478,13 +1478,13 @@
         <v>25</v>
       </c>
       <c r="D48" t="n">
-        <v>0.06430452986382033</v>
+        <v>0.1540991866939559</v>
       </c>
       <c r="E48" t="n">
-        <v>0.9356954701361797</v>
+        <v>0.8459008133060441</v>
       </c>
       <c r="F48" t="n">
-        <v>0.124969482421875</v>
+        <v>0.1292626857757568</v>
       </c>
     </row>
     <row r="49">
@@ -1500,13 +1500,13 @@
         <v>25</v>
       </c>
       <c r="D49" t="n">
-        <v>0.05271930898684834</v>
+        <v>0.08266495933029742</v>
       </c>
       <c r="E49" t="n">
-        <v>0.9472806910131517</v>
+        <v>0.9173350406697025</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1249687671661377</v>
+        <v>0.1231350898742676</v>
       </c>
     </row>
     <row r="50">
@@ -1522,13 +1522,13 @@
         <v>25</v>
       </c>
       <c r="D50" t="n">
-        <v>0.05188444053799679</v>
+        <v>0.04947470654360541</v>
       </c>
       <c r="E50" t="n">
-        <v>0.9481155594620032</v>
+        <v>0.9505252934563946</v>
       </c>
       <c r="F50" t="n">
-        <v>0.1249823570251465</v>
+        <v>0.121227502822876</v>
       </c>
     </row>
     <row r="51">
@@ -1544,13 +1544,13 @@
         <v>25</v>
       </c>
       <c r="D51" t="n">
-        <v>0.04121466048265078</v>
+        <v>0.1580199287590554</v>
       </c>
       <c r="E51" t="n">
-        <v>0.9587853395173491</v>
+        <v>0.8419800712409446</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1249585151672363</v>
+        <v>0.1226353645324707</v>
       </c>
     </row>
     <row r="52">
@@ -1566,13 +1566,13 @@
         <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>0.015</v>
+        <v>0.1</v>
       </c>
       <c r="E52" t="n">
-        <v>0.985</v>
+        <v>0.9</v>
       </c>
       <c r="F52" t="n">
-        <v>0.2176263332366943</v>
+        <v>0.2321817874908447</v>
       </c>
     </row>
     <row r="53">
@@ -1588,13 +1588,13 @@
         <v>25</v>
       </c>
       <c r="D53" t="n">
-        <v>0.007</v>
+        <v>0.024</v>
       </c>
       <c r="E53" t="n">
-        <v>0.993</v>
+        <v>0.976</v>
       </c>
       <c r="F53" t="n">
-        <v>0.2186999320983887</v>
+        <v>0.2120361328125</v>
       </c>
     </row>
     <row r="54">
@@ -1610,13 +1610,13 @@
         <v>25</v>
       </c>
       <c r="D54" t="n">
-        <v>0.036</v>
+        <v>0.018</v>
       </c>
       <c r="E54" t="n">
-        <v>0.964</v>
+        <v>0.982</v>
       </c>
       <c r="F54" t="n">
-        <v>0.2186992168426514</v>
+        <v>0.2235965728759766</v>
       </c>
     </row>
     <row r="55">
@@ -1632,13 +1632,13 @@
         <v>25</v>
       </c>
       <c r="D55" t="n">
-        <v>0.011</v>
+        <v>0.021</v>
       </c>
       <c r="E55" t="n">
-        <v>0.989</v>
+        <v>0.979</v>
       </c>
       <c r="F55" t="n">
-        <v>0.2186567783355713</v>
+        <v>0.2219018936157227</v>
       </c>
     </row>
     <row r="56">
@@ -1654,13 +1654,13 @@
         <v>25</v>
       </c>
       <c r="D56" t="n">
-        <v>0.015</v>
+        <v>0.033</v>
       </c>
       <c r="E56" t="n">
-        <v>0.985</v>
+        <v>0.967</v>
       </c>
       <c r="F56" t="n">
-        <v>0.2343604564666748</v>
+        <v>0.2213282585144043</v>
       </c>
     </row>
     <row r="57">
@@ -1676,13 +1676,13 @@
         <v>25</v>
       </c>
       <c r="D57" t="n">
-        <v>0.042</v>
+        <v>0.032</v>
       </c>
       <c r="E57" t="n">
-        <v>0.958</v>
+        <v>0.968</v>
       </c>
       <c r="F57" t="n">
-        <v>0.218698263168335</v>
+        <v>0.2145369052886963</v>
       </c>
     </row>
     <row r="58">
@@ -1698,13 +1698,13 @@
         <v>25</v>
       </c>
       <c r="D58" t="n">
-        <v>0.027</v>
+        <v>0.049</v>
       </c>
       <c r="E58" t="n">
-        <v>0.973</v>
+        <v>0.951</v>
       </c>
       <c r="F58" t="n">
-        <v>0.2186996936798096</v>
+        <v>0.2231652736663818</v>
       </c>
     </row>
     <row r="59">
@@ -1720,13 +1720,13 @@
         <v>25</v>
       </c>
       <c r="D59" t="n">
-        <v>0.048</v>
+        <v>0.029</v>
       </c>
       <c r="E59" t="n">
-        <v>0.952</v>
+        <v>0.971</v>
       </c>
       <c r="F59" t="n">
-        <v>0.2186968326568604</v>
+        <v>0.2123236656188965</v>
       </c>
     </row>
     <row r="60">
@@ -1742,13 +1742,13 @@
         <v>25</v>
       </c>
       <c r="D60" t="n">
-        <v>0.034</v>
+        <v>0.044</v>
       </c>
       <c r="E60" t="n">
-        <v>0.966</v>
+        <v>0.956</v>
       </c>
       <c r="F60" t="n">
-        <v>0.2186996936798096</v>
+        <v>0.2227077484130859</v>
       </c>
     </row>
     <row r="61">
@@ -1764,13 +1764,13 @@
         <v>25</v>
       </c>
       <c r="D61" t="n">
-        <v>0.015</v>
+        <v>0.025</v>
       </c>
       <c r="E61" t="n">
-        <v>0.985</v>
+        <v>0.975</v>
       </c>
       <c r="F61" t="n">
-        <v>0.2186977863311768</v>
+        <v>0.2230141162872314</v>
       </c>
     </row>
     <row r="62">
@@ -1786,13 +1786,13 @@
         <v>25</v>
       </c>
       <c r="D62" t="n">
-        <v>0.018</v>
+        <v>0.032</v>
       </c>
       <c r="E62" t="n">
-        <v>0.982</v>
+        <v>0.968</v>
       </c>
       <c r="F62" t="n">
-        <v>0.2187004089355469</v>
+        <v>0.2205381393432617</v>
       </c>
     </row>
     <row r="63">
@@ -1808,13 +1808,13 @@
         <v>25</v>
       </c>
       <c r="D63" t="n">
-        <v>0.004</v>
+        <v>0.035</v>
       </c>
       <c r="E63" t="n">
-        <v>0.996</v>
+        <v>0.965</v>
       </c>
       <c r="F63" t="n">
-        <v>0.2186963558197021</v>
+        <v>0.2149536609649658</v>
       </c>
     </row>
     <row r="64">
@@ -1830,13 +1830,13 @@
         <v>25</v>
       </c>
       <c r="D64" t="n">
-        <v>0.011</v>
+        <v>0.008</v>
       </c>
       <c r="E64" t="n">
-        <v>0.989</v>
+        <v>0.992</v>
       </c>
       <c r="F64" t="n">
-        <v>0.2186996936798096</v>
+        <v>0.220203161239624</v>
       </c>
     </row>
     <row r="65">
@@ -1852,13 +1852,13 @@
         <v>25</v>
       </c>
       <c r="D65" t="n">
-        <v>0.034</v>
+        <v>0.007</v>
       </c>
       <c r="E65" t="n">
-        <v>0.966</v>
+        <v>0.993</v>
       </c>
       <c r="F65" t="n">
-        <v>0.2187025547027588</v>
+        <v>0.2160243988037109</v>
       </c>
     </row>
     <row r="66">
@@ -1874,13 +1874,13 @@
         <v>25</v>
       </c>
       <c r="D66" t="n">
-        <v>0.055</v>
+        <v>0.046</v>
       </c>
       <c r="E66" t="n">
-        <v>0.945</v>
+        <v>0.954</v>
       </c>
       <c r="F66" t="n">
-        <v>0.2186946868896484</v>
+        <v>0.2202432155609131</v>
       </c>
     </row>
     <row r="67">
@@ -1896,13 +1896,13 @@
         <v>25</v>
       </c>
       <c r="D67" t="n">
-        <v>0.04</v>
+        <v>0.004</v>
       </c>
       <c r="E67" t="n">
-        <v>0.96</v>
+        <v>0.996</v>
       </c>
       <c r="F67" t="n">
-        <v>0.2186949253082275</v>
+        <v>0.2144284248352051</v>
       </c>
     </row>
     <row r="68">
@@ -1918,13 +1918,13 @@
         <v>25</v>
       </c>
       <c r="D68" t="n">
-        <v>0.062</v>
+        <v>0.007</v>
       </c>
       <c r="E68" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.993</v>
       </c>
       <c r="F68" t="n">
-        <v>0.2187016010284424</v>
+        <v>0.2209608554840088</v>
       </c>
     </row>
     <row r="69">
@@ -1940,13 +1940,13 @@
         <v>25</v>
       </c>
       <c r="D69" t="n">
-        <v>0.034</v>
+        <v>0.039</v>
       </c>
       <c r="E69" t="n">
-        <v>0.966</v>
+        <v>0.961</v>
       </c>
       <c r="F69" t="n">
-        <v>0.2186934947967529</v>
+        <v>0.214641809463501</v>
       </c>
     </row>
     <row r="70">
@@ -1962,13 +1962,13 @@
         <v>25</v>
       </c>
       <c r="D70" t="n">
-        <v>0.004</v>
+        <v>0.042</v>
       </c>
       <c r="E70" t="n">
-        <v>0.996</v>
+        <v>0.958</v>
       </c>
       <c r="F70" t="n">
-        <v>0.2187039852142334</v>
+        <v>0.2127666473388672</v>
       </c>
     </row>
     <row r="71">
@@ -1984,13 +1984,13 @@
         <v>25</v>
       </c>
       <c r="D71" t="n">
-        <v>0.014</v>
+        <v>0.051</v>
       </c>
       <c r="E71" t="n">
-        <v>0.986</v>
+        <v>0.949</v>
       </c>
       <c r="F71" t="n">
-        <v>0.2186985015869141</v>
+        <v>0.2124302387237549</v>
       </c>
     </row>
     <row r="72">
@@ -2006,13 +2006,13 @@
         <v>25</v>
       </c>
       <c r="D72" t="n">
-        <v>0.011</v>
+        <v>0.007</v>
       </c>
       <c r="E72" t="n">
-        <v>0.989</v>
+        <v>0.993</v>
       </c>
       <c r="F72" t="n">
-        <v>0.2186682224273682</v>
+        <v>0.2206451892852783</v>
       </c>
     </row>
     <row r="73">
@@ -2028,13 +2028,13 @@
         <v>25</v>
       </c>
       <c r="D73" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
       <c r="E73" t="n">
-        <v>0.999</v>
+        <v>0.99</v>
       </c>
       <c r="F73" t="n">
-        <v>0.2187278270721436</v>
+        <v>0.2143115997314453</v>
       </c>
     </row>
     <row r="74">
@@ -2050,13 +2050,13 @@
         <v>25</v>
       </c>
       <c r="D74" t="n">
-        <v>0.047</v>
+        <v>0.011</v>
       </c>
       <c r="E74" t="n">
-        <v>0.953</v>
+        <v>0.989</v>
       </c>
       <c r="F74" t="n">
-        <v>0.2186999320983887</v>
+        <v>0.2226026058197021</v>
       </c>
     </row>
     <row r="75">
@@ -2072,13 +2072,13 @@
         <v>25</v>
       </c>
       <c r="D75" t="n">
-        <v>0.06</v>
+        <v>0.035</v>
       </c>
       <c r="E75" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.965</v>
       </c>
       <c r="F75" t="n">
-        <v>0.2186975479125977</v>
+        <v>0.2212669849395752</v>
       </c>
     </row>
     <row r="76">
@@ -2094,13 +2094,13 @@
         <v>25</v>
       </c>
       <c r="D76" t="n">
-        <v>0.023</v>
+        <v>0.015</v>
       </c>
       <c r="E76" t="n">
-        <v>0.977</v>
+        <v>0.985</v>
       </c>
       <c r="F76" t="n">
-        <v>0.218698263168335</v>
+        <v>0.2144355773925781</v>
       </c>
     </row>
     <row r="77">
@@ -2116,13 +2116,13 @@
         <v>25</v>
       </c>
       <c r="D77" t="n">
-        <v>0.054</v>
+        <v>0.005</v>
       </c>
       <c r="E77" t="n">
-        <v>0.946</v>
+        <v>0.995</v>
       </c>
       <c r="F77" t="n">
-        <v>0.2187032699584961</v>
+        <v>0.2306535243988037</v>
       </c>
     </row>
     <row r="78">
@@ -2138,13 +2138,13 @@
         <v>25</v>
       </c>
       <c r="D78" t="n">
-        <v>0.14</v>
+        <v>0.089</v>
       </c>
       <c r="E78" t="n">
-        <v>0.86</v>
+        <v>0.911</v>
       </c>
       <c r="F78" t="n">
-        <v>0.2186946868896484</v>
+        <v>0.2255809307098389</v>
       </c>
     </row>
     <row r="79">
@@ -2160,13 +2160,13 @@
         <v>25</v>
       </c>
       <c r="D79" t="n">
-        <v>0.097</v>
+        <v>0.043</v>
       </c>
       <c r="E79" t="n">
-        <v>0.903</v>
+        <v>0.957</v>
       </c>
       <c r="F79" t="n">
-        <v>0.2186968326568604</v>
+        <v>0.2226386070251465</v>
       </c>
     </row>
     <row r="80">
@@ -2182,13 +2182,13 @@
         <v>25</v>
       </c>
       <c r="D80" t="n">
-        <v>0.081</v>
+        <v>0.09</v>
       </c>
       <c r="E80" t="n">
-        <v>0.919</v>
+        <v>0.91</v>
       </c>
       <c r="F80" t="n">
-        <v>0.2186756134033203</v>
+        <v>0.2127439975738525</v>
       </c>
     </row>
     <row r="81">
@@ -2204,13 +2204,13 @@
         <v>25</v>
       </c>
       <c r="D81" t="n">
-        <v>0.051</v>
+        <v>0.105</v>
       </c>
       <c r="E81" t="n">
-        <v>0.949</v>
+        <v>0.895</v>
       </c>
       <c r="F81" t="n">
-        <v>0.2187271118164062</v>
+        <v>0.2305450439453125</v>
       </c>
     </row>
     <row r="82">
@@ -2226,13 +2226,13 @@
         <v>25</v>
       </c>
       <c r="D82" t="n">
-        <v>0.062</v>
+        <v>0.055</v>
       </c>
       <c r="E82" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.945</v>
       </c>
       <c r="F82" t="n">
-        <v>0.2343146800994873</v>
+        <v>0.2252681255340576</v>
       </c>
     </row>
     <row r="83">
@@ -2248,13 +2248,13 @@
         <v>25</v>
       </c>
       <c r="D83" t="n">
-        <v>0.014</v>
+        <v>0.049</v>
       </c>
       <c r="E83" t="n">
-        <v>0.986</v>
+        <v>0.951</v>
       </c>
       <c r="F83" t="n">
-        <v>0.2186958789825439</v>
+        <v>0.2226309776306152</v>
       </c>
     </row>
     <row r="84">
@@ -2270,13 +2270,13 @@
         <v>25</v>
       </c>
       <c r="D84" t="n">
-        <v>0.053</v>
+        <v>0.025</v>
       </c>
       <c r="E84" t="n">
-        <v>0.947</v>
+        <v>0.975</v>
       </c>
       <c r="F84" t="n">
-        <v>0.2186994552612305</v>
+        <v>0.2225003242492676</v>
       </c>
     </row>
     <row r="85">
@@ -2292,13 +2292,13 @@
         <v>25</v>
       </c>
       <c r="D85" t="n">
-        <v>0.067</v>
+        <v>0.011</v>
       </c>
       <c r="E85" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.989</v>
       </c>
       <c r="F85" t="n">
-        <v>0.2186884880065918</v>
+        <v>0.2203586101531982</v>
       </c>
     </row>
     <row r="86">
@@ -2314,13 +2314,13 @@
         <v>25</v>
       </c>
       <c r="D86" t="n">
-        <v>0.025</v>
+        <v>0.204</v>
       </c>
       <c r="E86" t="n">
-        <v>0.975</v>
+        <v>0.796</v>
       </c>
       <c r="F86" t="n">
-        <v>0.2343347072601318</v>
+        <v>0.2226083278656006</v>
       </c>
     </row>
     <row r="87">
@@ -2336,13 +2336,13 @@
         <v>25</v>
       </c>
       <c r="D87" t="n">
-        <v>0.046</v>
+        <v>0.032</v>
       </c>
       <c r="E87" t="n">
-        <v>0.954</v>
+        <v>0.968</v>
       </c>
       <c r="F87" t="n">
-        <v>0.2186968326568604</v>
+        <v>0.2256736755371094</v>
       </c>
     </row>
     <row r="88">
@@ -2358,13 +2358,13 @@
         <v>25</v>
       </c>
       <c r="D88" t="n">
-        <v>0.024</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="E88" t="n">
-        <v>0.976</v>
+        <v>0.914</v>
       </c>
       <c r="F88" t="n">
-        <v>0.2186980247497559</v>
+        <v>0.2229914665222168</v>
       </c>
     </row>
     <row r="89">
@@ -2380,13 +2380,13 @@
         <v>25</v>
       </c>
       <c r="D89" t="n">
-        <v>0.006</v>
+        <v>0.028</v>
       </c>
       <c r="E89" t="n">
-        <v>0.994</v>
+        <v>0.972</v>
       </c>
       <c r="F89" t="n">
-        <v>0.2186987400054932</v>
+        <v>0.2289786338806152</v>
       </c>
     </row>
     <row r="90">
@@ -2402,13 +2402,13 @@
         <v>25</v>
       </c>
       <c r="D90" t="n">
-        <v>0.147</v>
+        <v>0.041</v>
       </c>
       <c r="E90" t="n">
-        <v>0.853</v>
+        <v>0.959</v>
       </c>
       <c r="F90" t="n">
-        <v>0.2186973094940186</v>
+        <v>0.2219440937042236</v>
       </c>
     </row>
     <row r="91">
@@ -2424,13 +2424,13 @@
         <v>25</v>
       </c>
       <c r="D91" t="n">
-        <v>0.013</v>
+        <v>0.082</v>
       </c>
       <c r="E91" t="n">
-        <v>0.987</v>
+        <v>0.918</v>
       </c>
       <c r="F91" t="n">
-        <v>0.2343204021453857</v>
+        <v>0.2149612903594971</v>
       </c>
     </row>
     <row r="92">
@@ -2446,13 +2446,13 @@
         <v>25</v>
       </c>
       <c r="D92" t="n">
-        <v>0.026</v>
+        <v>0.12</v>
       </c>
       <c r="E92" t="n">
-        <v>0.974</v>
+        <v>0.88</v>
       </c>
       <c r="F92" t="n">
-        <v>0.2187047004699707</v>
+        <v>0.2152845859527588</v>
       </c>
     </row>
     <row r="93">
@@ -2468,13 +2468,13 @@
         <v>25</v>
       </c>
       <c r="D93" t="n">
-        <v>0.13</v>
+        <v>0.032</v>
       </c>
       <c r="E93" t="n">
-        <v>0.87</v>
+        <v>0.968</v>
       </c>
       <c r="F93" t="n">
-        <v>0.2186963558197021</v>
+        <v>0.2274487018585205</v>
       </c>
     </row>
     <row r="94">
@@ -2490,13 +2490,13 @@
         <v>25</v>
       </c>
       <c r="D94" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.023</v>
       </c>
       <c r="E94" t="n">
-        <v>0.928</v>
+        <v>0.977</v>
       </c>
       <c r="F94" t="n">
-        <v>0.2186839580535889</v>
+        <v>0.2252717018127441</v>
       </c>
     </row>
     <row r="95">
@@ -2512,13 +2512,13 @@
         <v>25</v>
       </c>
       <c r="D95" t="n">
-        <v>0.043</v>
+        <v>0.082</v>
       </c>
       <c r="E95" t="n">
-        <v>0.957</v>
+        <v>0.918</v>
       </c>
       <c r="F95" t="n">
-        <v>0.2187089920043945</v>
+        <v>0.2353429794311523</v>
       </c>
     </row>
     <row r="96">
@@ -2534,13 +2534,13 @@
         <v>25</v>
       </c>
       <c r="D96" t="n">
-        <v>0.033</v>
+        <v>0.063</v>
       </c>
       <c r="E96" t="n">
-        <v>0.967</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="F96" t="n">
-        <v>0.2187001705169678</v>
+        <v>0.2153041362762451</v>
       </c>
     </row>
     <row r="97">
@@ -2556,13 +2556,13 @@
         <v>25</v>
       </c>
       <c r="D97" t="n">
-        <v>0.12</v>
+        <v>0.064</v>
       </c>
       <c r="E97" t="n">
-        <v>0.88</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="F97" t="n">
-        <v>0.2343196868896484</v>
+        <v>0.225306510925293</v>
       </c>
     </row>
     <row r="98">
@@ -2578,13 +2578,13 @@
         <v>25</v>
       </c>
       <c r="D98" t="n">
-        <v>0.016</v>
+        <v>0.007</v>
       </c>
       <c r="E98" t="n">
-        <v>0.984</v>
+        <v>0.993</v>
       </c>
       <c r="F98" t="n">
-        <v>0.2186965942382812</v>
+        <v>0.2228319644927979</v>
       </c>
     </row>
     <row r="99">
@@ -2600,13 +2600,13 @@
         <v>25</v>
       </c>
       <c r="D99" t="n">
-        <v>0.059</v>
+        <v>0.04</v>
       </c>
       <c r="E99" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="F99" t="n">
-        <v>0.2187049388885498</v>
+        <v>0.2349913120269775</v>
       </c>
     </row>
     <row r="100">
@@ -2622,13 +2622,13 @@
         <v>25</v>
       </c>
       <c r="D100" t="n">
-        <v>0.065</v>
+        <v>0.113</v>
       </c>
       <c r="E100" t="n">
-        <v>0.9350000000000001</v>
+        <v>0.887</v>
       </c>
       <c r="F100" t="n">
-        <v>0.2186932563781738</v>
+        <v>0.216094970703125</v>
       </c>
     </row>
     <row r="101">
@@ -2644,13 +2644,13 @@
         <v>25</v>
       </c>
       <c r="D101" t="n">
-        <v>0.065</v>
+        <v>0.003</v>
       </c>
       <c r="E101" t="n">
-        <v>0.9350000000000001</v>
+        <v>0.997</v>
       </c>
       <c r="F101" t="n">
-        <v>0.2186999320983887</v>
+        <v>0.225783109664917</v>
       </c>
     </row>
     <row r="102">
@@ -2666,13 +2666,13 @@
         <v>25</v>
       </c>
       <c r="D102" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E102" t="n">
-        <v>0.975024975024975</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F102" t="n">
-        <v>20.828125</v>
+        <v>42.515625</v>
       </c>
     </row>
     <row r="103">
@@ -2688,13 +2688,13 @@
         <v>25</v>
       </c>
       <c r="D103" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E103" t="n">
-        <v>0.967032967032967</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F103" t="n">
-        <v>22.109375</v>
+        <v>43.21875</v>
       </c>
     </row>
     <row r="104">
@@ -2710,13 +2710,13 @@
         <v>25</v>
       </c>
       <c r="D104" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="E104" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.98001998001998</v>
       </c>
       <c r="F104" t="n">
-        <v>21.671875</v>
+        <v>42.640625</v>
       </c>
     </row>
     <row r="105">
@@ -2732,13 +2732,13 @@
         <v>25</v>
       </c>
       <c r="D105" t="n">
-        <v>0.01898101898101898</v>
+        <v>0.01598401598401598</v>
       </c>
       <c r="E105" t="n">
-        <v>0.981018981018981</v>
+        <v>0.984015984015984</v>
       </c>
       <c r="F105" t="n">
-        <v>21.59375</v>
+        <v>41.828125</v>
       </c>
     </row>
     <row r="106">
@@ -2754,13 +2754,13 @@
         <v>25</v>
       </c>
       <c r="D106" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.01398601398601399</v>
       </c>
       <c r="E106" t="n">
-        <v>0.977022977022977</v>
+        <v>0.986013986013986</v>
       </c>
       <c r="F106" t="n">
-        <v>21.78125</v>
+        <v>41.6875</v>
       </c>
     </row>
     <row r="107">
@@ -2776,13 +2776,13 @@
         <v>25</v>
       </c>
       <c r="D107" t="n">
-        <v>0.03596403596403597</v>
+        <v>0.01598401598401598</v>
       </c>
       <c r="E107" t="n">
-        <v>0.964035964035964</v>
+        <v>0.984015984015984</v>
       </c>
       <c r="F107" t="n">
-        <v>21.84375</v>
+        <v>41.90625</v>
       </c>
     </row>
     <row r="108">
@@ -2798,13 +2798,13 @@
         <v>25</v>
       </c>
       <c r="D108" t="n">
-        <v>0.03896103896103896</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E108" t="n">
-        <v>0.961038961038961</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F108" t="n">
-        <v>21.796875</v>
+        <v>42.78125</v>
       </c>
     </row>
     <row r="109">
@@ -2820,13 +2820,13 @@
         <v>25</v>
       </c>
       <c r="D109" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E109" t="n">
-        <v>0.965034965034965</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F109" t="n">
-        <v>21.484375</v>
+        <v>41.375</v>
       </c>
     </row>
     <row r="110">
@@ -2842,13 +2842,13 @@
         <v>25</v>
       </c>
       <c r="D110" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="E110" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.98001998001998</v>
       </c>
       <c r="F110" t="n">
-        <v>21.234375</v>
+        <v>42.5625</v>
       </c>
     </row>
     <row r="111">
@@ -2864,13 +2864,13 @@
         <v>25</v>
       </c>
       <c r="D111" t="n">
-        <v>0.03996003996003996</v>
+        <v>0.03596403596403597</v>
       </c>
       <c r="E111" t="n">
-        <v>0.9600399600399601</v>
+        <v>0.964035964035964</v>
       </c>
       <c r="F111" t="n">
-        <v>21.3125</v>
+        <v>43.265625</v>
       </c>
     </row>
     <row r="112">
@@ -2886,13 +2886,13 @@
         <v>25</v>
       </c>
       <c r="D112" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E112" t="n">
-        <v>0.97002997002997</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F112" t="n">
-        <v>22.28125</v>
+        <v>42.71875</v>
       </c>
     </row>
     <row r="113">
@@ -2908,13 +2908,13 @@
         <v>25</v>
       </c>
       <c r="D113" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="E113" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.98001998001998</v>
       </c>
       <c r="F113" t="n">
-        <v>21.375</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114">
@@ -2930,13 +2930,13 @@
         <v>25</v>
       </c>
       <c r="D114" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.01198801198801199</v>
       </c>
       <c r="E114" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.988011988011988</v>
       </c>
       <c r="F114" t="n">
-        <v>22.125</v>
+        <v>41</v>
       </c>
     </row>
     <row r="115">
@@ -2952,13 +2952,13 @@
         <v>25</v>
       </c>
       <c r="D115" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.01598401598401598</v>
       </c>
       <c r="E115" t="n">
-        <v>0.971028971028971</v>
+        <v>0.984015984015984</v>
       </c>
       <c r="F115" t="n">
-        <v>21.734375</v>
+        <v>42.859375</v>
       </c>
     </row>
     <row r="116">
@@ -2974,13 +2974,13 @@
         <v>25</v>
       </c>
       <c r="D116" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.01598401598401598</v>
       </c>
       <c r="E116" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.984015984015984</v>
       </c>
       <c r="F116" t="n">
-        <v>21.90625</v>
+        <v>42.90625</v>
       </c>
     </row>
     <row r="117">
@@ -2996,13 +2996,13 @@
         <v>25</v>
       </c>
       <c r="D117" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.01598401598401598</v>
       </c>
       <c r="E117" t="n">
-        <v>0.977022977022977</v>
+        <v>0.984015984015984</v>
       </c>
       <c r="F117" t="n">
-        <v>21.453125</v>
+        <v>44.65625</v>
       </c>
     </row>
     <row r="118">
@@ -3018,13 +3018,13 @@
         <v>25</v>
       </c>
       <c r="D118" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E118" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F118" t="n">
-        <v>21.609375</v>
+        <v>42.65625</v>
       </c>
     </row>
     <row r="119">
@@ -3040,13 +3040,13 @@
         <v>25</v>
       </c>
       <c r="D119" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E119" t="n">
-        <v>0.975024975024975</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F119" t="n">
-        <v>21.875</v>
+        <v>44.078125</v>
       </c>
     </row>
     <row r="120">
@@ -3062,13 +3062,13 @@
         <v>25</v>
       </c>
       <c r="D120" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E120" t="n">
-        <v>0.965034965034965</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F120" t="n">
-        <v>22.28125</v>
+        <v>42.84375</v>
       </c>
     </row>
     <row r="121">
@@ -3084,13 +3084,13 @@
         <v>25</v>
       </c>
       <c r="D121" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.02297702297702298</v>
       </c>
       <c r="E121" t="n">
-        <v>0.965034965034965</v>
+        <v>0.977022977022977</v>
       </c>
       <c r="F121" t="n">
-        <v>22.390625</v>
+        <v>42.484375</v>
       </c>
     </row>
     <row r="122">
@@ -3106,13 +3106,13 @@
         <v>25</v>
       </c>
       <c r="D122" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E122" t="n">
-        <v>0.977022977022977</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F122" t="n">
-        <v>22.09375</v>
+        <v>43.40625</v>
       </c>
     </row>
     <row r="123">
@@ -3128,13 +3128,13 @@
         <v>25</v>
       </c>
       <c r="D123" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E123" t="n">
-        <v>0.967032967032967</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F123" t="n">
-        <v>21.78125</v>
+        <v>41.3125</v>
       </c>
     </row>
     <row r="124">
@@ -3150,13 +3150,13 @@
         <v>25</v>
       </c>
       <c r="D124" t="n">
-        <v>0.01698301698301698</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E124" t="n">
-        <v>0.983016983016983</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F124" t="n">
-        <v>21.78125</v>
+        <v>44.234375</v>
       </c>
     </row>
     <row r="125">
@@ -3172,13 +3172,13 @@
         <v>25</v>
       </c>
       <c r="D125" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.005994005994005994</v>
       </c>
       <c r="E125" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.994005994005994</v>
       </c>
       <c r="F125" t="n">
-        <v>21.578125</v>
+        <v>41.71875</v>
       </c>
     </row>
     <row r="126">
@@ -3200,7 +3200,7 @@
         <v>0.971028971028971</v>
       </c>
       <c r="F126" t="n">
-        <v>21.34375</v>
+        <v>42.78125</v>
       </c>
     </row>
     <row r="127">
@@ -3216,13 +3216,13 @@
         <v>25</v>
       </c>
       <c r="D127" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.03196803196803197</v>
       </c>
       <c r="E127" t="n">
-        <v>0.967032967032967</v>
+        <v>0.968031968031968</v>
       </c>
       <c r="F127" t="n">
-        <v>22.328125</v>
+        <v>41.6875</v>
       </c>
     </row>
     <row r="128">
@@ -3238,13 +3238,13 @@
         <v>25</v>
       </c>
       <c r="D128" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.03596403596403597</v>
       </c>
       <c r="E128" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.964035964035964</v>
       </c>
       <c r="F128" t="n">
-        <v>21.625</v>
+        <v>44</v>
       </c>
     </row>
     <row r="129">
@@ -3260,13 +3260,13 @@
         <v>25</v>
       </c>
       <c r="D129" t="n">
-        <v>0.02597402597402598</v>
+        <v>0.03896103896103896</v>
       </c>
       <c r="E129" t="n">
-        <v>0.974025974025974</v>
+        <v>0.961038961038961</v>
       </c>
       <c r="F129" t="n">
-        <v>22.859375</v>
+        <v>45.171875</v>
       </c>
     </row>
     <row r="130">
@@ -3288,7 +3288,7 @@
         <v>0.9690309690309691</v>
       </c>
       <c r="F130" t="n">
-        <v>23.046875</v>
+        <v>43.21875</v>
       </c>
     </row>
     <row r="131">
@@ -3304,13 +3304,13 @@
         <v>25</v>
       </c>
       <c r="D131" t="n">
-        <v>0.04295704295704296</v>
+        <v>0.02397602397602398</v>
       </c>
       <c r="E131" t="n">
-        <v>0.9570429570429571</v>
+        <v>0.9760239760239761</v>
       </c>
       <c r="F131" t="n">
-        <v>21.875</v>
+        <v>42.53125</v>
       </c>
     </row>
     <row r="132">
@@ -3326,13 +3326,13 @@
         <v>25</v>
       </c>
       <c r="D132" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.02497502497502498</v>
       </c>
       <c r="E132" t="n">
-        <v>0.965034965034965</v>
+        <v>0.975024975024975</v>
       </c>
       <c r="F132" t="n">
-        <v>22.0625</v>
+        <v>45.0625</v>
       </c>
     </row>
     <row r="133">
@@ -3348,13 +3348,13 @@
         <v>25</v>
       </c>
       <c r="D133" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.03496503496503497</v>
       </c>
       <c r="E133" t="n">
-        <v>0.972027972027972</v>
+        <v>0.965034965034965</v>
       </c>
       <c r="F133" t="n">
-        <v>22.34375</v>
+        <v>42.3125</v>
       </c>
     </row>
     <row r="134">
@@ -3370,13 +3370,13 @@
         <v>25</v>
       </c>
       <c r="D134" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.01898101898101898</v>
       </c>
       <c r="E134" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.981018981018981</v>
       </c>
       <c r="F134" t="n">
-        <v>22.375</v>
+        <v>43.609375</v>
       </c>
     </row>
     <row r="135">
@@ -3392,13 +3392,13 @@
         <v>25</v>
       </c>
       <c r="D135" t="n">
-        <v>0.02597402597402598</v>
+        <v>0.03996003996003996</v>
       </c>
       <c r="E135" t="n">
-        <v>0.974025974025974</v>
+        <v>0.9600399600399601</v>
       </c>
       <c r="F135" t="n">
-        <v>21.640625</v>
+        <v>44.828125</v>
       </c>
     </row>
     <row r="136">
@@ -3414,13 +3414,13 @@
         <v>25</v>
       </c>
       <c r="D136" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.03596403596403597</v>
       </c>
       <c r="E136" t="n">
-        <v>0.967032967032967</v>
+        <v>0.964035964035964</v>
       </c>
       <c r="F136" t="n">
-        <v>22.265625</v>
+        <v>43.515625</v>
       </c>
     </row>
     <row r="137">
@@ -3436,13 +3436,13 @@
         <v>25</v>
       </c>
       <c r="D137" t="n">
-        <v>0.04195804195804196</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E137" t="n">
-        <v>0.958041958041958</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F137" t="n">
-        <v>22.8125</v>
+        <v>42.984375</v>
       </c>
     </row>
     <row r="138">
@@ -3458,13 +3458,13 @@
         <v>25</v>
       </c>
       <c r="D138" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.02397602397602398</v>
       </c>
       <c r="E138" t="n">
-        <v>0.97002997002997</v>
+        <v>0.9760239760239761</v>
       </c>
       <c r="F138" t="n">
-        <v>22.1875</v>
+        <v>43.796875</v>
       </c>
     </row>
     <row r="139">
@@ -3480,13 +3480,13 @@
         <v>25</v>
       </c>
       <c r="D139" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.03596403596403597</v>
       </c>
       <c r="E139" t="n">
-        <v>0.97002997002997</v>
+        <v>0.964035964035964</v>
       </c>
       <c r="F139" t="n">
-        <v>21.875</v>
+        <v>44.421875</v>
       </c>
     </row>
     <row r="140">
@@ -3502,13 +3502,13 @@
         <v>25</v>
       </c>
       <c r="D140" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E140" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F140" t="n">
-        <v>23.453125</v>
+        <v>46.546875</v>
       </c>
     </row>
     <row r="141">
@@ -3524,13 +3524,13 @@
         <v>25</v>
       </c>
       <c r="D141" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E141" t="n">
-        <v>0.975024975024975</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F141" t="n">
-        <v>23.390625</v>
+        <v>44.015625</v>
       </c>
     </row>
     <row r="142">
@@ -3546,13 +3546,13 @@
         <v>25</v>
       </c>
       <c r="D142" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E142" t="n">
-        <v>0.968031968031968</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F142" t="n">
-        <v>22.0625</v>
+        <v>46.046875</v>
       </c>
     </row>
     <row r="143">
@@ -3568,13 +3568,13 @@
         <v>25</v>
       </c>
       <c r="D143" t="n">
-        <v>0.02197802197802198</v>
+        <v>0.02497502497502498</v>
       </c>
       <c r="E143" t="n">
-        <v>0.978021978021978</v>
+        <v>0.975024975024975</v>
       </c>
       <c r="F143" t="n">
-        <v>21.78125</v>
+        <v>43.046875</v>
       </c>
     </row>
     <row r="144">
@@ -3590,13 +3590,13 @@
         <v>25</v>
       </c>
       <c r="D144" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E144" t="n">
-        <v>0.968031968031968</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F144" t="n">
-        <v>21.953125</v>
+        <v>44.265625</v>
       </c>
     </row>
     <row r="145">
@@ -3612,13 +3612,13 @@
         <v>25</v>
       </c>
       <c r="D145" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.02997002997002997</v>
       </c>
       <c r="E145" t="n">
-        <v>0.975024975024975</v>
+        <v>0.97002997002997</v>
       </c>
       <c r="F145" t="n">
-        <v>22.140625</v>
+        <v>42.890625</v>
       </c>
     </row>
     <row r="146">
@@ -3634,13 +3634,13 @@
         <v>25</v>
       </c>
       <c r="D146" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E146" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F146" t="n">
-        <v>22.5</v>
+        <v>45.203125</v>
       </c>
     </row>
     <row r="147">
@@ -3656,13 +3656,13 @@
         <v>25</v>
       </c>
       <c r="D147" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E147" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F147" t="n">
-        <v>21.984375</v>
+        <v>44.25</v>
       </c>
     </row>
     <row r="148">
@@ -3678,13 +3678,13 @@
         <v>25</v>
       </c>
       <c r="D148" t="n">
-        <v>0.04395604395604396</v>
+        <v>0.02497502497502498</v>
       </c>
       <c r="E148" t="n">
-        <v>0.9560439560439561</v>
+        <v>0.975024975024975</v>
       </c>
       <c r="F148" t="n">
-        <v>23.171875</v>
+        <v>42.96875</v>
       </c>
     </row>
     <row r="149">
@@ -3700,13 +3700,13 @@
         <v>25</v>
       </c>
       <c r="D149" t="n">
-        <v>0.04195804195804196</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E149" t="n">
-        <v>0.958041958041958</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F149" t="n">
-        <v>22.609375</v>
+        <v>44.734375</v>
       </c>
     </row>
     <row r="150">
@@ -3722,13 +3722,13 @@
         <v>25</v>
       </c>
       <c r="D150" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.03496503496503497</v>
       </c>
       <c r="E150" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.965034965034965</v>
       </c>
       <c r="F150" t="n">
-        <v>21.421875</v>
+        <v>43.90625</v>
       </c>
     </row>
     <row r="151">
@@ -3744,13 +3744,13 @@
         <v>25</v>
       </c>
       <c r="D151" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E151" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F151" t="n">
-        <v>21.734375</v>
+        <v>43.28125</v>
       </c>
     </row>
     <row r="152">
@@ -3766,13 +3766,13 @@
         <v>25</v>
       </c>
       <c r="D152" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E152" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F152" t="n">
-        <v>23.84375</v>
+        <v>48.15625</v>
       </c>
     </row>
     <row r="153">
@@ -3788,13 +3788,13 @@
         <v>25</v>
       </c>
       <c r="D153" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E153" t="n">
-        <v>0.972027972027972</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F153" t="n">
-        <v>24.125</v>
+        <v>48.21875</v>
       </c>
     </row>
     <row r="154">
@@ -3810,13 +3810,13 @@
         <v>25</v>
       </c>
       <c r="D154" t="n">
-        <v>0.01998001998001998</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E154" t="n">
-        <v>0.98001998001998</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F154" t="n">
-        <v>24.9375</v>
+        <v>48.515625</v>
       </c>
     </row>
     <row r="155">
@@ -3832,13 +3832,13 @@
         <v>25</v>
       </c>
       <c r="D155" t="n">
-        <v>0.01998001998001998</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E155" t="n">
-        <v>0.98001998001998</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F155" t="n">
-        <v>25.078125</v>
+        <v>48.375</v>
       </c>
     </row>
     <row r="156">
@@ -3854,13 +3854,13 @@
         <v>25</v>
       </c>
       <c r="D156" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.01298701298701299</v>
       </c>
       <c r="E156" t="n">
-        <v>0.968031968031968</v>
+        <v>0.987012987012987</v>
       </c>
       <c r="F156" t="n">
-        <v>24.671875</v>
+        <v>48.265625</v>
       </c>
     </row>
     <row r="157">
@@ -3876,13 +3876,13 @@
         <v>25</v>
       </c>
       <c r="D157" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E157" t="n">
-        <v>0.972027972027972</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F157" t="n">
-        <v>25.0625</v>
+        <v>47.859375</v>
       </c>
     </row>
     <row r="158">
@@ -3898,13 +3898,13 @@
         <v>25</v>
       </c>
       <c r="D158" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E158" t="n">
-        <v>0.965034965034965</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F158" t="n">
-        <v>25.03125</v>
+        <v>49.125</v>
       </c>
     </row>
     <row r="159">
@@ -3920,13 +3920,13 @@
         <v>25</v>
       </c>
       <c r="D159" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.01498501498501499</v>
       </c>
       <c r="E159" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.985014985014985</v>
       </c>
       <c r="F159" t="n">
-        <v>24.84375</v>
+        <v>48.765625</v>
       </c>
     </row>
     <row r="160">
@@ -3942,13 +3942,13 @@
         <v>25</v>
       </c>
       <c r="D160" t="n">
-        <v>0.02597402597402598</v>
+        <v>0.02297702297702298</v>
       </c>
       <c r="E160" t="n">
-        <v>0.974025974025974</v>
+        <v>0.977022977022977</v>
       </c>
       <c r="F160" t="n">
-        <v>25.0625</v>
+        <v>49.515625</v>
       </c>
     </row>
     <row r="161">
@@ -3964,13 +3964,13 @@
         <v>25</v>
       </c>
       <c r="D161" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.01298701298701299</v>
       </c>
       <c r="E161" t="n">
-        <v>0.971028971028971</v>
+        <v>0.987012987012987</v>
       </c>
       <c r="F161" t="n">
-        <v>25.203125</v>
+        <v>49.84375</v>
       </c>
     </row>
     <row r="162">
@@ -3986,13 +3986,13 @@
         <v>25</v>
       </c>
       <c r="D162" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E162" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F162" t="n">
-        <v>25.125</v>
+        <v>48.609375</v>
       </c>
     </row>
     <row r="163">
@@ -4008,13 +4008,13 @@
         <v>25</v>
       </c>
       <c r="D163" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E163" t="n">
-        <v>0.968031968031968</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F163" t="n">
-        <v>24.703125</v>
+        <v>48.3125</v>
       </c>
     </row>
     <row r="164">
@@ -4030,13 +4030,13 @@
         <v>25</v>
       </c>
       <c r="D164" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.02297702297702298</v>
       </c>
       <c r="E164" t="n">
-        <v>0.968031968031968</v>
+        <v>0.977022977022977</v>
       </c>
       <c r="F164" t="n">
-        <v>25.375</v>
+        <v>49.046875</v>
       </c>
     </row>
     <row r="165">
@@ -4052,13 +4052,13 @@
         <v>25</v>
       </c>
       <c r="D165" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.01598401598401598</v>
       </c>
       <c r="E165" t="n">
-        <v>0.971028971028971</v>
+        <v>0.984015984015984</v>
       </c>
       <c r="F165" t="n">
-        <v>24.828125</v>
+        <v>50.234375</v>
       </c>
     </row>
     <row r="166">
@@ -4074,13 +4074,13 @@
         <v>25</v>
       </c>
       <c r="D166" t="n">
-        <v>0.02597402597402598</v>
+        <v>0.01698301698301698</v>
       </c>
       <c r="E166" t="n">
-        <v>0.974025974025974</v>
+        <v>0.983016983016983</v>
       </c>
       <c r="F166" t="n">
-        <v>24.828125</v>
+        <v>48.265625</v>
       </c>
     </row>
     <row r="167">
@@ -4096,13 +4096,13 @@
         <v>25</v>
       </c>
       <c r="D167" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E167" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F167" t="n">
-        <v>24.765625</v>
+        <v>48.8125</v>
       </c>
     </row>
     <row r="168">
@@ -4118,13 +4118,13 @@
         <v>25</v>
       </c>
       <c r="D168" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E168" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F168" t="n">
-        <v>25.078125</v>
+        <v>49.03125</v>
       </c>
     </row>
     <row r="169">
@@ -4140,13 +4140,13 @@
         <v>25</v>
       </c>
       <c r="D169" t="n">
-        <v>0.02597402597402598</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E169" t="n">
-        <v>0.974025974025974</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F169" t="n">
-        <v>24.796875</v>
+        <v>48.46875</v>
       </c>
     </row>
     <row r="170">
@@ -4168,7 +4168,7 @@
         <v>0.9790209790209791</v>
       </c>
       <c r="F170" t="n">
-        <v>24.703125</v>
+        <v>48.71875</v>
       </c>
     </row>
     <row r="171">
@@ -4184,13 +4184,13 @@
         <v>25</v>
       </c>
       <c r="D171" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E171" t="n">
-        <v>0.97002997002997</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F171" t="n">
-        <v>24.828125</v>
+        <v>49.734375</v>
       </c>
     </row>
     <row r="172">
@@ -4206,13 +4206,13 @@
         <v>25</v>
       </c>
       <c r="D172" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.01698301698301698</v>
       </c>
       <c r="E172" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.983016983016983</v>
       </c>
       <c r="F172" t="n">
-        <v>24.796875</v>
+        <v>48.890625</v>
       </c>
     </row>
     <row r="173">
@@ -4228,13 +4228,13 @@
         <v>25</v>
       </c>
       <c r="D173" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E173" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F173" t="n">
-        <v>24.390625</v>
+        <v>48.359375</v>
       </c>
     </row>
     <row r="174">
@@ -4250,13 +4250,13 @@
         <v>25</v>
       </c>
       <c r="D174" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E174" t="n">
-        <v>0.977022977022977</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F174" t="n">
-        <v>23.890625</v>
+        <v>48.96875</v>
       </c>
     </row>
     <row r="175">
@@ -4272,13 +4272,13 @@
         <v>25</v>
       </c>
       <c r="D175" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.01498501498501499</v>
       </c>
       <c r="E175" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.985014985014985</v>
       </c>
       <c r="F175" t="n">
-        <v>24.953125</v>
+        <v>47.703125</v>
       </c>
     </row>
     <row r="176">
@@ -4294,13 +4294,13 @@
         <v>25</v>
       </c>
       <c r="D176" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E176" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F176" t="n">
-        <v>23.609375</v>
+        <v>46.59375</v>
       </c>
     </row>
     <row r="177">
@@ -4316,13 +4316,13 @@
         <v>25</v>
       </c>
       <c r="D177" t="n">
-        <v>0.05194805194805195</v>
+        <v>0.03396603396603397</v>
       </c>
       <c r="E177" t="n">
-        <v>0.948051948051948</v>
+        <v>0.9660339660339661</v>
       </c>
       <c r="F177" t="n">
-        <v>25.34375</v>
+        <v>50.234375</v>
       </c>
     </row>
     <row r="178">
@@ -4338,13 +4338,13 @@
         <v>25</v>
       </c>
       <c r="D178" t="n">
-        <v>0.02597402597402598</v>
+        <v>0.03596403596403597</v>
       </c>
       <c r="E178" t="n">
-        <v>0.974025974025974</v>
+        <v>0.964035964035964</v>
       </c>
       <c r="F178" t="n">
-        <v>25.5</v>
+        <v>49.15625</v>
       </c>
     </row>
     <row r="179">
@@ -4360,13 +4360,13 @@
         <v>25</v>
       </c>
       <c r="D179" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.03796203796203796</v>
       </c>
       <c r="E179" t="n">
-        <v>0.97002997002997</v>
+        <v>0.962037962037962</v>
       </c>
       <c r="F179" t="n">
-        <v>25.109375</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="180">
@@ -4382,13 +4382,13 @@
         <v>25</v>
       </c>
       <c r="D180" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E180" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F180" t="n">
-        <v>25.171875</v>
+        <v>49.21875</v>
       </c>
     </row>
     <row r="181">
@@ -4404,13 +4404,13 @@
         <v>25</v>
       </c>
       <c r="D181" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.03096903096903097</v>
       </c>
       <c r="E181" t="n">
-        <v>0.965034965034965</v>
+        <v>0.9690309690309691</v>
       </c>
       <c r="F181" t="n">
-        <v>25.078125</v>
+        <v>49.25</v>
       </c>
     </row>
     <row r="182">
@@ -4426,13 +4426,13 @@
         <v>25</v>
       </c>
       <c r="D182" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.03796203796203796</v>
       </c>
       <c r="E182" t="n">
-        <v>0.971028971028971</v>
+        <v>0.962037962037962</v>
       </c>
       <c r="F182" t="n">
-        <v>25.34375</v>
+        <v>50.234375</v>
       </c>
     </row>
     <row r="183">
@@ -4448,13 +4448,13 @@
         <v>25</v>
       </c>
       <c r="D183" t="n">
-        <v>0.04395604395604396</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E183" t="n">
-        <v>0.9560439560439561</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F183" t="n">
-        <v>25.90625</v>
+        <v>49.90625</v>
       </c>
     </row>
     <row r="184">
@@ -4470,13 +4470,13 @@
         <v>25</v>
       </c>
       <c r="D184" t="n">
-        <v>0.03596403596403597</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E184" t="n">
-        <v>0.964035964035964</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F184" t="n">
-        <v>25.40625</v>
+        <v>50.0625</v>
       </c>
     </row>
     <row r="185">
@@ -4492,13 +4492,13 @@
         <v>25</v>
       </c>
       <c r="D185" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E185" t="n">
-        <v>0.975024975024975</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F185" t="n">
-        <v>25.703125</v>
+        <v>50.078125</v>
       </c>
     </row>
     <row r="186">
@@ -4514,13 +4514,13 @@
         <v>25</v>
       </c>
       <c r="D186" t="n">
-        <v>0.03796203796203796</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E186" t="n">
-        <v>0.962037962037962</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F186" t="n">
-        <v>25.0625</v>
+        <v>49.609375</v>
       </c>
     </row>
     <row r="187">
@@ -4536,13 +4536,13 @@
         <v>25</v>
       </c>
       <c r="D187" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E187" t="n">
-        <v>0.97002997002997</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F187" t="n">
-        <v>25.546875</v>
+        <v>49.484375</v>
       </c>
     </row>
     <row r="188">
@@ -4558,13 +4558,13 @@
         <v>25</v>
       </c>
       <c r="D188" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.03496503496503497</v>
       </c>
       <c r="E188" t="n">
-        <v>0.967032967032967</v>
+        <v>0.965034965034965</v>
       </c>
       <c r="F188" t="n">
-        <v>25.90625</v>
+        <v>49.46875</v>
       </c>
     </row>
     <row r="189">
@@ -4580,13 +4580,13 @@
         <v>25</v>
       </c>
       <c r="D189" t="n">
-        <v>0.03596403596403597</v>
+        <v>0.04095904095904096</v>
       </c>
       <c r="E189" t="n">
-        <v>0.964035964035964</v>
+        <v>0.9590409590409591</v>
       </c>
       <c r="F189" t="n">
-        <v>25.734375</v>
+        <v>50.140625</v>
       </c>
     </row>
     <row r="190">
@@ -4602,13 +4602,13 @@
         <v>25</v>
       </c>
       <c r="D190" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E190" t="n">
-        <v>0.967032967032967</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F190" t="n">
-        <v>25.375</v>
+        <v>50.25</v>
       </c>
     </row>
     <row r="191">
@@ -4624,13 +4624,13 @@
         <v>25</v>
       </c>
       <c r="D191" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E191" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F191" t="n">
-        <v>25.1875</v>
+        <v>49.609375</v>
       </c>
     </row>
     <row r="192">
@@ -4646,13 +4646,13 @@
         <v>25</v>
       </c>
       <c r="D192" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.02397602397602398</v>
       </c>
       <c r="E192" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.9760239760239761</v>
       </c>
       <c r="F192" t="n">
-        <v>25.453125</v>
+        <v>49.703125</v>
       </c>
     </row>
     <row r="193">
@@ -4668,13 +4668,13 @@
         <v>25</v>
       </c>
       <c r="D193" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.03096903096903097</v>
       </c>
       <c r="E193" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.9690309690309691</v>
       </c>
       <c r="F193" t="n">
-        <v>25.203125</v>
+        <v>49.890625</v>
       </c>
     </row>
     <row r="194">
@@ -4690,13 +4690,13 @@
         <v>25</v>
       </c>
       <c r="D194" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.03696303696303696</v>
       </c>
       <c r="E194" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.9630369630369631</v>
       </c>
       <c r="F194" t="n">
-        <v>25.4375</v>
+        <v>50.4375</v>
       </c>
     </row>
     <row r="195">
@@ -4712,13 +4712,13 @@
         <v>25</v>
       </c>
       <c r="D195" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.02997002997002997</v>
       </c>
       <c r="E195" t="n">
-        <v>0.968031968031968</v>
+        <v>0.97002997002997</v>
       </c>
       <c r="F195" t="n">
-        <v>24.921875</v>
+        <v>49.921875</v>
       </c>
     </row>
     <row r="196">
@@ -4734,13 +4734,13 @@
         <v>25</v>
       </c>
       <c r="D196" t="n">
-        <v>0.04495504495504495</v>
+        <v>0.03096903096903097</v>
       </c>
       <c r="E196" t="n">
-        <v>0.955044955044955</v>
+        <v>0.9690309690309691</v>
       </c>
       <c r="F196" t="n">
-        <v>26.078125</v>
+        <v>48.90625</v>
       </c>
     </row>
     <row r="197">
@@ -4756,13 +4756,13 @@
         <v>25</v>
       </c>
       <c r="D197" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.03396603396603397</v>
       </c>
       <c r="E197" t="n">
-        <v>0.975024975024975</v>
+        <v>0.9660339660339661</v>
       </c>
       <c r="F197" t="n">
-        <v>25.09375</v>
+        <v>48.96875</v>
       </c>
     </row>
     <row r="198">
@@ -4778,13 +4778,13 @@
         <v>25</v>
       </c>
       <c r="D198" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E198" t="n">
-        <v>0.971028971028971</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F198" t="n">
-        <v>25.21875</v>
+        <v>49.328125</v>
       </c>
     </row>
     <row r="199">
@@ -4800,13 +4800,13 @@
         <v>25</v>
       </c>
       <c r="D199" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E199" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F199" t="n">
-        <v>24.703125</v>
+        <v>47.921875</v>
       </c>
     </row>
     <row r="200">
@@ -4822,13 +4822,13 @@
         <v>25</v>
       </c>
       <c r="D200" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.02497502497502498</v>
       </c>
       <c r="E200" t="n">
-        <v>0.968031968031968</v>
+        <v>0.975024975024975</v>
       </c>
       <c r="F200" t="n">
-        <v>24.109375</v>
+        <v>46.828125</v>
       </c>
     </row>
     <row r="201">
@@ -4844,13 +4844,13 @@
         <v>25</v>
       </c>
       <c r="D201" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.02997002997002997</v>
       </c>
       <c r="E201" t="n">
-        <v>0.972027972027972</v>
+        <v>0.97002997002997</v>
       </c>
       <c r="F201" t="n">
-        <v>23.765625</v>
+        <v>48.265625</v>
       </c>
     </row>
     <row r="202">
@@ -4866,13 +4866,13 @@
         <v>25</v>
       </c>
       <c r="D202" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E202" t="n">
-        <v>0.977022977022977</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F202" t="n">
-        <v>27.84375</v>
+        <v>54.546875</v>
       </c>
     </row>
     <row r="203">
@@ -4888,13 +4888,13 @@
         <v>25</v>
       </c>
       <c r="D203" t="n">
-        <v>0.02197802197802198</v>
+        <v>0.01898101898101898</v>
       </c>
       <c r="E203" t="n">
-        <v>0.978021978021978</v>
+        <v>0.981018981018981</v>
       </c>
       <c r="F203" t="n">
-        <v>27.703125</v>
+        <v>53.953125</v>
       </c>
     </row>
     <row r="204">
@@ -4910,13 +4910,13 @@
         <v>25</v>
       </c>
       <c r="D204" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.01498501498501499</v>
       </c>
       <c r="E204" t="n">
-        <v>0.972027972027972</v>
+        <v>0.985014985014985</v>
       </c>
       <c r="F204" t="n">
-        <v>28.15625</v>
+        <v>54.171875</v>
       </c>
     </row>
     <row r="205">
@@ -4932,13 +4932,13 @@
         <v>25</v>
       </c>
       <c r="D205" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.02397602397602398</v>
       </c>
       <c r="E205" t="n">
-        <v>0.977022977022977</v>
+        <v>0.9760239760239761</v>
       </c>
       <c r="F205" t="n">
-        <v>27.6875</v>
+        <v>54.828125</v>
       </c>
     </row>
     <row r="206">
@@ -4954,13 +4954,13 @@
         <v>25</v>
       </c>
       <c r="D206" t="n">
-        <v>0.02297702297702298</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E206" t="n">
-        <v>0.977022977022977</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F206" t="n">
-        <v>27.8125</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="207">
@@ -4982,7 +4982,7 @@
         <v>0.975024975024975</v>
       </c>
       <c r="F207" t="n">
-        <v>27.953125</v>
+        <v>54.875</v>
       </c>
     </row>
     <row r="208">
@@ -4998,13 +4998,13 @@
         <v>25</v>
       </c>
       <c r="D208" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.01898101898101898</v>
       </c>
       <c r="E208" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.981018981018981</v>
       </c>
       <c r="F208" t="n">
-        <v>27.75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="209">
@@ -5020,13 +5020,13 @@
         <v>25</v>
       </c>
       <c r="D209" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E209" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F209" t="n">
-        <v>27.765625</v>
+        <v>54.421875</v>
       </c>
     </row>
     <row r="210">
@@ -5042,13 +5042,13 @@
         <v>25</v>
       </c>
       <c r="D210" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.01398601398601399</v>
       </c>
       <c r="E210" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.986013986013986</v>
       </c>
       <c r="F210" t="n">
-        <v>28.5625</v>
+        <v>55.046875</v>
       </c>
     </row>
     <row r="211">
@@ -5064,13 +5064,13 @@
         <v>25</v>
       </c>
       <c r="D211" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E211" t="n">
-        <v>0.975024975024975</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F211" t="n">
-        <v>27.78125</v>
+        <v>54.609375</v>
       </c>
     </row>
     <row r="212">
@@ -5086,13 +5086,13 @@
         <v>25</v>
       </c>
       <c r="D212" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.01398601398601399</v>
       </c>
       <c r="E212" t="n">
-        <v>0.968031968031968</v>
+        <v>0.986013986013986</v>
       </c>
       <c r="F212" t="n">
-        <v>27.9375</v>
+        <v>54.109375</v>
       </c>
     </row>
     <row r="213">
@@ -5108,13 +5108,13 @@
         <v>25</v>
       </c>
       <c r="D213" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.01098901098901099</v>
       </c>
       <c r="E213" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.9890109890109891</v>
       </c>
       <c r="F213" t="n">
-        <v>27.671875</v>
+        <v>55.796875</v>
       </c>
     </row>
     <row r="214">
@@ -5130,13 +5130,13 @@
         <v>25</v>
       </c>
       <c r="D214" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="E214" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.98001998001998</v>
       </c>
       <c r="F214" t="n">
-        <v>27.671875</v>
+        <v>54.609375</v>
       </c>
     </row>
     <row r="215">
@@ -5152,13 +5152,13 @@
         <v>25</v>
       </c>
       <c r="D215" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.02097902097902098</v>
       </c>
       <c r="E215" t="n">
-        <v>0.97002997002997</v>
+        <v>0.9790209790209791</v>
       </c>
       <c r="F215" t="n">
-        <v>27.671875</v>
+        <v>54.734375</v>
       </c>
     </row>
     <row r="216">
@@ -5174,13 +5174,13 @@
         <v>25</v>
       </c>
       <c r="D216" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.01498501498501499</v>
       </c>
       <c r="E216" t="n">
-        <v>0.97002997002997</v>
+        <v>0.985014985014985</v>
       </c>
       <c r="F216" t="n">
-        <v>27.625</v>
+        <v>54.796875</v>
       </c>
     </row>
     <row r="217">
@@ -5196,13 +5196,13 @@
         <v>25</v>
       </c>
       <c r="D217" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.02297702297702298</v>
       </c>
       <c r="E217" t="n">
-        <v>0.972027972027972</v>
+        <v>0.977022977022977</v>
       </c>
       <c r="F217" t="n">
-        <v>27.734375</v>
+        <v>54.484375</v>
       </c>
     </row>
     <row r="218">
@@ -5218,13 +5218,13 @@
         <v>25</v>
       </c>
       <c r="D218" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="E218" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.98001998001998</v>
       </c>
       <c r="F218" t="n">
-        <v>27.921875</v>
+        <v>54.4375</v>
       </c>
     </row>
     <row r="219">
@@ -5240,13 +5240,13 @@
         <v>25</v>
       </c>
       <c r="D219" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.02297702297702298</v>
       </c>
       <c r="E219" t="n">
-        <v>0.97002997002997</v>
+        <v>0.977022977022977</v>
       </c>
       <c r="F219" t="n">
-        <v>27.8125</v>
+        <v>55.171875</v>
       </c>
     </row>
     <row r="220">
@@ -5262,13 +5262,13 @@
         <v>25</v>
       </c>
       <c r="D220" t="n">
-        <v>0.02997002997002997</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="E220" t="n">
-        <v>0.97002997002997</v>
+        <v>0.98001998001998</v>
       </c>
       <c r="F220" t="n">
-        <v>27.5625</v>
+        <v>54.234375</v>
       </c>
     </row>
     <row r="221">
@@ -5284,13 +5284,13 @@
         <v>25</v>
       </c>
       <c r="D221" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.01398601398601399</v>
       </c>
       <c r="E221" t="n">
-        <v>0.9730269730269731</v>
+        <v>0.986013986013986</v>
       </c>
       <c r="F221" t="n">
-        <v>27.546875</v>
+        <v>54.8125</v>
       </c>
     </row>
     <row r="222">
@@ -5306,13 +5306,13 @@
         <v>25</v>
       </c>
       <c r="D222" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E222" t="n">
-        <v>0.975024975024975</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F222" t="n">
-        <v>27.875</v>
+        <v>54.625</v>
       </c>
     </row>
     <row r="223">
@@ -5328,13 +5328,13 @@
         <v>25</v>
       </c>
       <c r="D223" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.01898101898101898</v>
       </c>
       <c r="E223" t="n">
-        <v>0.972027972027972</v>
+        <v>0.981018981018981</v>
       </c>
       <c r="F223" t="n">
-        <v>27.6875</v>
+        <v>53.28125</v>
       </c>
     </row>
     <row r="224">
@@ -5350,13 +5350,13 @@
         <v>25</v>
       </c>
       <c r="D224" t="n">
-        <v>0.04295704295704296</v>
+        <v>0.02297702297702298</v>
       </c>
       <c r="E224" t="n">
-        <v>0.9570429570429571</v>
+        <v>0.977022977022977</v>
       </c>
       <c r="F224" t="n">
-        <v>27.390625</v>
+        <v>53.96875</v>
       </c>
     </row>
     <row r="225">
@@ -5372,13 +5372,13 @@
         <v>25</v>
       </c>
       <c r="D225" t="n">
-        <v>0.02097902097902098</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E225" t="n">
-        <v>0.9790209790209791</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F225" t="n">
-        <v>27.84375</v>
+        <v>53.90625</v>
       </c>
     </row>
     <row r="226">
@@ -5394,13 +5394,13 @@
         <v>25</v>
       </c>
       <c r="D226" t="n">
-        <v>0.02097902097902098</v>
+        <v>0.01798201798201798</v>
       </c>
       <c r="E226" t="n">
-        <v>0.9790209790209791</v>
+        <v>0.9820179820179821</v>
       </c>
       <c r="F226" t="n">
-        <v>26.46875</v>
+        <v>50.703125</v>
       </c>
     </row>
     <row r="227">
@@ -5422,7 +5422,7 @@
         <v>0.971028971028971</v>
       </c>
       <c r="F227" t="n">
-        <v>28.5</v>
+        <v>56.140625</v>
       </c>
     </row>
     <row r="228">
@@ -5438,13 +5438,13 @@
         <v>25</v>
       </c>
       <c r="D228" t="n">
-        <v>0.03496503496503497</v>
+        <v>0.03196803196803197</v>
       </c>
       <c r="E228" t="n">
-        <v>0.965034965034965</v>
+        <v>0.968031968031968</v>
       </c>
       <c r="F228" t="n">
-        <v>28.46875</v>
+        <v>55.625</v>
       </c>
     </row>
     <row r="229">
@@ -5460,13 +5460,13 @@
         <v>25</v>
       </c>
       <c r="D229" t="n">
-        <v>0.03596403596403597</v>
+        <v>0.03896103896103896</v>
       </c>
       <c r="E229" t="n">
-        <v>0.964035964035964</v>
+        <v>0.961038961038961</v>
       </c>
       <c r="F229" t="n">
-        <v>28.53125</v>
+        <v>54.453125</v>
       </c>
     </row>
     <row r="230">
@@ -5482,13 +5482,13 @@
         <v>25</v>
       </c>
       <c r="D230" t="n">
-        <v>0.03596403596403597</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E230" t="n">
-        <v>0.964035964035964</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F230" t="n">
-        <v>28.484375</v>
+        <v>55.421875</v>
       </c>
     </row>
     <row r="231">
@@ -5504,13 +5504,13 @@
         <v>25</v>
       </c>
       <c r="D231" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E231" t="n">
-        <v>0.968031968031968</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F231" t="n">
-        <v>28.515625</v>
+        <v>55.140625</v>
       </c>
     </row>
     <row r="232">
@@ -5526,13 +5526,13 @@
         <v>25</v>
       </c>
       <c r="D232" t="n">
-        <v>0.02797202797202797</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E232" t="n">
-        <v>0.972027972027972</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F232" t="n">
-        <v>28.765625</v>
+        <v>56.734375</v>
       </c>
     </row>
     <row r="233">
@@ -5548,13 +5548,13 @@
         <v>25</v>
       </c>
       <c r="D233" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E233" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F233" t="n">
-        <v>28.65625</v>
+        <v>56.1875</v>
       </c>
     </row>
     <row r="234">
@@ -5570,13 +5570,13 @@
         <v>25</v>
       </c>
       <c r="D234" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.03196803196803197</v>
       </c>
       <c r="E234" t="n">
-        <v>0.971028971028971</v>
+        <v>0.968031968031968</v>
       </c>
       <c r="F234" t="n">
-        <v>28.1875</v>
+        <v>55.8125</v>
       </c>
     </row>
     <row r="235">
@@ -5592,13 +5592,13 @@
         <v>25</v>
       </c>
       <c r="D235" t="n">
-        <v>0.03696303696303696</v>
+        <v>0.02697302697302697</v>
       </c>
       <c r="E235" t="n">
-        <v>0.9630369630369631</v>
+        <v>0.9730269730269731</v>
       </c>
       <c r="F235" t="n">
-        <v>28.984375</v>
+        <v>55.765625</v>
       </c>
     </row>
     <row r="236">
@@ -5614,13 +5614,13 @@
         <v>25</v>
       </c>
       <c r="D236" t="n">
-        <v>0.02497502497502498</v>
+        <v>0.01898101898101898</v>
       </c>
       <c r="E236" t="n">
-        <v>0.975024975024975</v>
+        <v>0.981018981018981</v>
       </c>
       <c r="F236" t="n">
-        <v>28.65625</v>
+        <v>56.359375</v>
       </c>
     </row>
     <row r="237">
@@ -5636,13 +5636,13 @@
         <v>25</v>
       </c>
       <c r="D237" t="n">
-        <v>0.03896103896103896</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E237" t="n">
-        <v>0.961038961038961</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F237" t="n">
-        <v>28.25</v>
+        <v>55.28125</v>
       </c>
     </row>
     <row r="238">
@@ -5658,13 +5658,13 @@
         <v>25</v>
       </c>
       <c r="D238" t="n">
-        <v>0.04195804195804196</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="E238" t="n">
-        <v>0.958041958041958</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F238" t="n">
-        <v>28.09375</v>
+        <v>55.46875</v>
       </c>
     </row>
     <row r="239">
@@ -5680,13 +5680,13 @@
         <v>25</v>
       </c>
       <c r="D239" t="n">
-        <v>0.03396603396603397</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="E239" t="n">
-        <v>0.9660339660339661</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="F239" t="n">
-        <v>28.859375</v>
+        <v>55.125</v>
       </c>
     </row>
     <row r="240">
@@ -5702,13 +5702,13 @@
         <v>25</v>
       </c>
       <c r="D240" t="n">
-        <v>0.03996003996003996</v>
+        <v>0.03296703296703297</v>
       </c>
       <c r="E240" t="n">
-        <v>0.9600399600399601</v>
+        <v>0.967032967032967</v>
       </c>
       <c r="F240" t="n">
-        <v>28.3125</v>
+        <v>56.4375</v>
       </c>
     </row>
     <row r="241">
@@ -5724,13 +5724,13 @@
         <v>25</v>
       </c>
       <c r="D241" t="n">
-        <v>0.02897102897102897</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E241" t="n">
-        <v>0.971028971028971</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F241" t="n">
-        <v>28.390625</v>
+        <v>55.296875</v>
       </c>
     </row>
     <row r="242">
@@ -5746,13 +5746,13 @@
         <v>25</v>
       </c>
       <c r="D242" t="n">
-        <v>0.04095904095904096</v>
+        <v>0.03296703296703297</v>
       </c>
       <c r="E242" t="n">
-        <v>0.9590409590409591</v>
+        <v>0.967032967032967</v>
       </c>
       <c r="F242" t="n">
-        <v>28.609375</v>
+        <v>54.6875</v>
       </c>
     </row>
     <row r="243">
@@ -5768,13 +5768,13 @@
         <v>25</v>
       </c>
       <c r="D243" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E243" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F243" t="n">
-        <v>28.359375</v>
+        <v>55.796875</v>
       </c>
     </row>
     <row r="244">
@@ -5790,13 +5790,13 @@
         <v>25</v>
       </c>
       <c r="D244" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.03596403596403597</v>
       </c>
       <c r="E244" t="n">
-        <v>0.967032967032967</v>
+        <v>0.964035964035964</v>
       </c>
       <c r="F244" t="n">
-        <v>28.484375</v>
+        <v>55.828125</v>
       </c>
     </row>
     <row r="245">
@@ -5812,13 +5812,13 @@
         <v>25</v>
       </c>
       <c r="D245" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.03896103896103896</v>
       </c>
       <c r="E245" t="n">
-        <v>0.967032967032967</v>
+        <v>0.961038961038961</v>
       </c>
       <c r="F245" t="n">
-        <v>28.578125</v>
+        <v>54.46875</v>
       </c>
     </row>
     <row r="246">
@@ -5834,13 +5834,13 @@
         <v>25</v>
       </c>
       <c r="D246" t="n">
-        <v>0.03196803196803197</v>
+        <v>0.04695304695304695</v>
       </c>
       <c r="E246" t="n">
-        <v>0.968031968031968</v>
+        <v>0.9530469530469531</v>
       </c>
       <c r="F246" t="n">
-        <v>28.1875</v>
+        <v>56.203125</v>
       </c>
     </row>
     <row r="247">
@@ -5856,13 +5856,13 @@
         <v>25</v>
       </c>
       <c r="D247" t="n">
-        <v>0.03996003996003996</v>
+        <v>0.03796203796203796</v>
       </c>
       <c r="E247" t="n">
-        <v>0.9600399600399601</v>
+        <v>0.962037962037962</v>
       </c>
       <c r="F247" t="n">
-        <v>28.34375</v>
+        <v>54.515625</v>
       </c>
     </row>
     <row r="248">
@@ -5878,13 +5878,13 @@
         <v>25</v>
       </c>
       <c r="D248" t="n">
-        <v>0.04495504495504495</v>
+        <v>0.02797202797202797</v>
       </c>
       <c r="E248" t="n">
-        <v>0.955044955044955</v>
+        <v>0.972027972027972</v>
       </c>
       <c r="F248" t="n">
-        <v>27.5625</v>
+        <v>55.921875</v>
       </c>
     </row>
     <row r="249">
@@ -5900,13 +5900,13 @@
         <v>25</v>
       </c>
       <c r="D249" t="n">
-        <v>0.03296703296703297</v>
+        <v>0.02997002997002997</v>
       </c>
       <c r="E249" t="n">
-        <v>0.967032967032967</v>
+        <v>0.97002997002997</v>
       </c>
       <c r="F249" t="n">
-        <v>27.640625</v>
+        <v>55.546875</v>
       </c>
     </row>
     <row r="250">
@@ -5922,13 +5922,13 @@
         <v>25</v>
       </c>
       <c r="D250" t="n">
-        <v>0.03096903096903097</v>
+        <v>0.03696303696303696</v>
       </c>
       <c r="E250" t="n">
-        <v>0.9690309690309691</v>
+        <v>0.9630369630369631</v>
       </c>
       <c r="F250" t="n">
-        <v>27.71875</v>
+        <v>54.78125</v>
       </c>
     </row>
     <row r="251">
@@ -5944,13 +5944,13 @@
         <v>25</v>
       </c>
       <c r="D251" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.02897102897102897</v>
       </c>
       <c r="E251" t="n">
-        <v>0.9760239760239761</v>
+        <v>0.971028971028971</v>
       </c>
       <c r="F251" t="n">
-        <v>27.140625</v>
+        <v>54.984375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>